<commit_message>
Count All Palindromic Subsequence
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\DSA-with-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F501A93-361B-4320-90E7-7D70B95B4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D098EA3-A5EA-44E4-9129-DD88FD0DDD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1632,16 +1632,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1653,7 +1644,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1974,17 +1974,17 @@
   <dimension ref="A1:F482"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2011,17 +2011,17 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="E6" s="14" t="s">
         <v>468</v>
       </c>
       <c r="F6" s="15" cm="1">
         <f t="array" ref="F6">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" outlineLevel="1">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" outlineLevel="1">
@@ -2435,11 +2435,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="1:3" ht="21" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2552,11 +2552,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
     </row>
     <row r="57" spans="1:3" ht="21" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -2797,7 +2797,7 @@
         <v>75</v>
       </c>
       <c r="C78" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="21" outlineLevel="1">
@@ -3032,11 +3032,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="23"/>
-      <c r="C101" s="23"/>
+      <c r="B101" s="16"/>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" spans="1:3" ht="21" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3435,11 +3435,11 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="19"/>
-      <c r="C139" s="19"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="20"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3838,11 +3838,11 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="23" t="s">
+      <c r="A177" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="23"/>
-      <c r="C177" s="23"/>
+      <c r="B177" s="16"/>
+      <c r="C177" s="16"/>
     </row>
     <row r="178" spans="1:3" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4235,11 +4235,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
     </row>
     <row r="215" spans="1:3" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4488,11 +4488,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="23" t="s">
+      <c r="A238" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="23"/>
-      <c r="C238" s="23"/>
+      <c r="B238" s="16"/>
+      <c r="C238" s="16"/>
     </row>
     <row r="239" spans="1:3" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4884,11 +4884,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="17"/>
+      <c r="C275" s="17"/>
     </row>
     <row r="276" spans="1:3" ht="21" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5104,11 +5104,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="23" t="s">
+      <c r="A296" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="B296" s="23"/>
-      <c r="C296" s="23"/>
+      <c r="B296" s="16"/>
+      <c r="C296" s="16"/>
     </row>
     <row r="297" spans="1:3" ht="21" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5533,11 +5533,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="17"/>
+      <c r="C336" s="17"/>
     </row>
     <row r="337" spans="1:3" ht="21" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5742,11 +5742,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="16" t="s">
+      <c r="A356" s="21" t="s">
         <v>467</v>
       </c>
-      <c r="B356" s="16"/>
-      <c r="C356" s="16"/>
+      <c r="B356" s="21"/>
+      <c r="C356" s="21"/>
     </row>
     <row r="357" spans="1:3" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6237,11 +6237,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="17" t="s">
+      <c r="A402" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="17"/>
-      <c r="C402" s="17"/>
+      <c r="B402" s="22"/>
+      <c r="C402" s="22"/>
     </row>
     <row r="403" spans="1:3" ht="21" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6314,11 +6314,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="18" t="s">
+      <c r="A410" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="18"/>
-      <c r="C410" s="18"/>
+      <c r="B410" s="23"/>
+      <c r="C410" s="23"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6985,11 +6985,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="19" t="s">
+      <c r="A472" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="19"/>
-      <c r="C472" s="19"/>
+      <c r="B472" s="20"/>
+      <c r="C472" s="20"/>
     </row>
     <row r="473" spans="1:3" ht="21" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7103,21 +7103,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Second Most Repeated String In An Array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910FA475-1DD2-4E03-82B8-C9EAD4149F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5BA12E-1C3E-4364-B9F9-78C8A92EC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1632,7 +1632,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1644,16 +1653,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1974,7 +1974,7 @@
   <dimension ref="A1:F482"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2011,17 +2011,17 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="E6" s="14" t="s">
         <v>468</v>
       </c>
       <c r="F6" s="15" cm="1">
         <f t="array" ref="F6">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" outlineLevel="1">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))</f>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" outlineLevel="1">
@@ -2435,11 +2435,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
     </row>
     <row r="45" spans="1:3" ht="21" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2552,11 +2552,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -2874,7 +2874,7 @@
         <v>82</v>
       </c>
       <c r="C85" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="21" outlineLevel="1">
@@ -3032,11 +3032,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="16"/>
-      <c r="C101" s="16"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
     </row>
     <row r="102" spans="1:3" ht="21" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3435,11 +3435,11 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="20" t="s">
+      <c r="A139" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="20"/>
-      <c r="C139" s="20"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="19"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3838,11 +3838,11 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="16" t="s">
+      <c r="A177" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="16"/>
-      <c r="C177" s="16"/>
+      <c r="B177" s="23"/>
+      <c r="C177" s="23"/>
     </row>
     <row r="178" spans="1:3" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4235,11 +4235,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="17" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="17"/>
-      <c r="C214" s="17"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4488,11 +4488,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="16" t="s">
+      <c r="A238" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="16"/>
-      <c r="C238" s="16"/>
+      <c r="B238" s="23"/>
+      <c r="C238" s="23"/>
     </row>
     <row r="239" spans="1:3" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4884,11 +4884,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="17" t="s">
+      <c r="A275" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="B275" s="17"/>
-      <c r="C275" s="17"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5104,11 +5104,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="16" t="s">
+      <c r="A296" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="B296" s="16"/>
-      <c r="C296" s="16"/>
+      <c r="B296" s="23"/>
+      <c r="C296" s="23"/>
     </row>
     <row r="297" spans="1:3" ht="21" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5533,11 +5533,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="17" t="s">
+      <c r="A336" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="B336" s="17"/>
-      <c r="C336" s="17"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5742,11 +5742,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="21" t="s">
+      <c r="A356" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="B356" s="21"/>
-      <c r="C356" s="21"/>
+      <c r="B356" s="16"/>
+      <c r="C356" s="16"/>
     </row>
     <row r="357" spans="1:3" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6237,11 +6237,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="22" t="s">
+      <c r="A402" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="22"/>
-      <c r="C402" s="22"/>
+      <c r="B402" s="17"/>
+      <c r="C402" s="17"/>
     </row>
     <row r="403" spans="1:3" ht="21" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6314,11 +6314,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="23" t="s">
+      <c r="A410" s="18" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="23"/>
-      <c r="C410" s="23"/>
+      <c r="B410" s="18"/>
+      <c r="C410" s="18"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6985,11 +6985,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="20" t="s">
+      <c r="A472" s="19" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="20"/>
-      <c r="C472" s="20"/>
+      <c r="B472" s="19"/>
+      <c r="C472" s="19"/>
     </row>
     <row r="473" spans="1:3" ht="21" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7103,21 +7103,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Minimum number of swaps for bracket balancing
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5BA12E-1C3E-4364-B9F9-78C8A92EC987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D509F71D-83BF-4544-AD33-EB4999DFEA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1632,16 +1632,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1653,7 +1644,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1973,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2011,17 +2011,17 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="E6" s="14" t="s">
         <v>468</v>
       </c>
       <c r="F6" s="15" cm="1">
         <f t="array" ref="F6">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" outlineLevel="1">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))</f>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" outlineLevel="1">
@@ -2435,11 +2435,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="1:3" ht="21" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2552,11 +2552,11 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
     </row>
     <row r="57" spans="1:3" ht="21" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -2885,7 +2885,7 @@
         <v>83</v>
       </c>
       <c r="C86" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="21" outlineLevel="1">
@@ -3032,11 +3032,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="23"/>
-      <c r="C101" s="23"/>
+      <c r="B101" s="16"/>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" spans="1:3" ht="21" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3435,11 +3435,11 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="19"/>
-      <c r="C139" s="19"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="20"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3838,11 +3838,11 @@
       </c>
     </row>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="23" t="s">
+      <c r="A177" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="23"/>
-      <c r="C177" s="23"/>
+      <c r="B177" s="16"/>
+      <c r="C177" s="16"/>
     </row>
     <row r="178" spans="1:3" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4235,11 +4235,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="17"/>
+      <c r="C214" s="17"/>
     </row>
     <row r="215" spans="1:3" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4488,11 +4488,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="23" t="s">
+      <c r="A238" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="23"/>
-      <c r="C238" s="23"/>
+      <c r="B238" s="16"/>
+      <c r="C238" s="16"/>
     </row>
     <row r="239" spans="1:3" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4884,11 +4884,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="17"/>
+      <c r="C275" s="17"/>
     </row>
     <row r="276" spans="1:3" ht="21" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5104,11 +5104,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="23" t="s">
+      <c r="A296" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="B296" s="23"/>
-      <c r="C296" s="23"/>
+      <c r="B296" s="16"/>
+      <c r="C296" s="16"/>
     </row>
     <row r="297" spans="1:3" ht="21" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5533,11 +5533,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="17"/>
+      <c r="C336" s="17"/>
     </row>
     <row r="337" spans="1:3" ht="21" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5742,11 +5742,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="16" t="s">
+      <c r="A356" s="21" t="s">
         <v>467</v>
       </c>
-      <c r="B356" s="16"/>
-      <c r="C356" s="16"/>
+      <c r="B356" s="21"/>
+      <c r="C356" s="21"/>
     </row>
     <row r="357" spans="1:3" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6237,11 +6237,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="17" t="s">
+      <c r="A402" s="22" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="17"/>
-      <c r="C402" s="17"/>
+      <c r="B402" s="22"/>
+      <c r="C402" s="22"/>
     </row>
     <row r="403" spans="1:3" ht="21" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6314,11 +6314,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="18" t="s">
+      <c r="A410" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="18"/>
-      <c r="C410" s="18"/>
+      <c r="B410" s="23"/>
+      <c r="C410" s="23"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6985,11 +6985,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="19" t="s">
+      <c r="A472" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="19"/>
-      <c r="C472" s="19"/>
+      <c r="B472" s="20"/>
+      <c r="C472" s="20"/>
     </row>
     <row r="473" spans="1:3" ht="21" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7103,21 +7103,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
N Meetings in Room
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9768B5DA-63A4-4F3E-99EA-159B3D3661DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97356589-CB80-4CED-875D-4A3FB36AA723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="A402" sqref="A402:C402"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4540,7 +4540,7 @@
       <c r="B238" s="26"/>
       <c r="C238" s="26"/>
     </row>
-    <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="239" spans="1:3" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
         <v>230</v>
       </c>
@@ -4548,10 +4548,10 @@
         <v>231</v>
       </c>
       <c r="C239" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="21" outlineLevel="1">
       <c r="A240" s="5" t="s">
         <v>230</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="241" spans="1:3" ht="21" outlineLevel="1">
       <c r="A241" s="5" t="s">
         <v>230</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="242" spans="1:3" ht="21" outlineLevel="1">
       <c r="A242" s="5" t="s">
         <v>230</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="243" spans="1:3" ht="21" outlineLevel="1">
       <c r="A243" s="5" t="s">
         <v>230</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="244" spans="1:3" ht="21" outlineLevel="1">
       <c r="A244" s="5" t="s">
         <v>230</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="245" spans="1:3" ht="21" outlineLevel="1">
       <c r="A245" s="5" t="s">
         <v>230</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="246" spans="1:3" ht="21" outlineLevel="1">
       <c r="A246" s="5" t="s">
         <v>230</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="247" spans="1:3" ht="21" outlineLevel="1">
       <c r="A247" s="5" t="s">
         <v>230</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="248" spans="1:3" ht="21" outlineLevel="1">
       <c r="A248" s="5" t="s">
         <v>230</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="249" spans="1:3" ht="21" outlineLevel="1">
       <c r="A249" s="5" t="s">
         <v>230</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="250" spans="1:3" ht="21" outlineLevel="1">
       <c r="A250" s="5" t="s">
         <v>230</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="251" spans="1:3" ht="21" outlineLevel="1">
       <c r="A251" s="5" t="s">
         <v>230</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="252" spans="1:3" ht="21" outlineLevel="1">
       <c r="A252" s="5" t="s">
         <v>230</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="253" spans="1:3" ht="21" outlineLevel="1">
       <c r="A253" s="5" t="s">
         <v>230</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="254" spans="1:3" ht="21" outlineLevel="1">
       <c r="A254" s="5" t="s">
         <v>230</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="255" spans="1:3" ht="21" outlineLevel="1">
       <c r="A255" s="5" t="s">
         <v>230</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="256" spans="1:3" ht="21" outlineLevel="1">
       <c r="A256" s="5" t="s">
         <v>230</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="257" spans="1:3" ht="21" outlineLevel="1">
       <c r="A257" s="5" t="s">
         <v>230</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="258" spans="1:3" ht="21" outlineLevel="1">
       <c r="A258" s="5" t="s">
         <v>230</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="259" spans="1:3" ht="21" outlineLevel="1">
       <c r="A259" s="5" t="s">
         <v>230</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="260" spans="1:3" ht="21" outlineLevel="1">
       <c r="A260" s="5" t="s">
         <v>230</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="261" spans="1:3" ht="21" outlineLevel="1">
       <c r="A261" s="5" t="s">
         <v>230</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="262" spans="1:3" ht="21" outlineLevel="1">
       <c r="A262" s="5" t="s">
         <v>230</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="263" spans="1:3" ht="21" outlineLevel="1">
       <c r="A263" s="5" t="s">
         <v>230</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="264" spans="1:3" ht="21" outlineLevel="1">
       <c r="A264" s="5" t="s">
         <v>230</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="265" spans="1:3" ht="21" outlineLevel="1">
       <c r="A265" s="5" t="s">
         <v>230</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="266" spans="1:3" ht="21" outlineLevel="1">
       <c r="A266" s="5" t="s">
         <v>230</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="267" spans="1:3" ht="21" outlineLevel="1">
       <c r="A267" s="5" t="s">
         <v>230</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="268" spans="1:3" ht="21" outlineLevel="1">
       <c r="A268" s="5" t="s">
         <v>230</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="269" spans="1:3" ht="21" outlineLevel="1">
       <c r="A269" s="5" t="s">
         <v>230</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="270" spans="1:3" ht="21" outlineLevel="1">
       <c r="A270" s="5" t="s">
         <v>230</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="271" spans="1:3" ht="21" outlineLevel="1">
       <c r="A271" s="5" t="s">
         <v>230</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="272" spans="1:3" ht="21" outlineLevel="1">
       <c r="A272" s="5" t="s">
         <v>230</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="273" spans="1:3" ht="21" outlineLevel="1">
       <c r="A273" s="5" t="s">
         <v>230</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="21" collapsed="1">
+    <row r="274" spans="1:3" ht="21">
       <c r="B274" s="7"/>
       <c r="C274" s="4"/>
     </row>
@@ -6366,7 +6366,7 @@
       <c r="B410" s="21"/>
       <c r="C410" s="21"/>
     </row>
-    <row r="411" spans="1:3" ht="21" outlineLevel="1">
+    <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
         <v>393</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="21" outlineLevel="1">
+    <row r="412" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A412" s="5" t="s">
         <v>393</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="21" outlineLevel="1">
+    <row r="413" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A413" s="5" t="s">
         <v>393</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="21" outlineLevel="1">
+    <row r="414" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A414" s="5" t="s">
         <v>393</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:3" ht="21" outlineLevel="1">
+    <row r="415" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A415" s="5" t="s">
         <v>393</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="21" outlineLevel="1">
+    <row r="416" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A416" s="5" t="s">
         <v>393</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="21" outlineLevel="1">
+    <row r="417" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A417" s="5" t="s">
         <v>393</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="21" outlineLevel="1">
+    <row r="418" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A418" s="5" t="s">
         <v>393</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="21" outlineLevel="1">
+    <row r="419" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A419" s="5" t="s">
         <v>393</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="21" outlineLevel="1">
+    <row r="420" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A420" s="5" t="s">
         <v>393</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="21" outlineLevel="1">
+    <row r="421" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A421" s="5" t="s">
         <v>393</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="21" outlineLevel="1">
+    <row r="422" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A422" s="5" t="s">
         <v>393</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="21" outlineLevel="1">
+    <row r="423" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A423" s="5" t="s">
         <v>393</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="21" outlineLevel="1">
+    <row r="424" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A424" s="5" t="s">
         <v>393</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="21" outlineLevel="1">
+    <row r="425" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A425" s="5" t="s">
         <v>393</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="21" outlineLevel="1">
+    <row r="426" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A426" s="5" t="s">
         <v>393</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="21" outlineLevel="1">
+    <row r="427" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A427" s="5" t="s">
         <v>393</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="21" outlineLevel="1">
+    <row r="428" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A428" s="5" t="s">
         <v>393</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="21" outlineLevel="1">
+    <row r="429" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A429" s="5" t="s">
         <v>393</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="21" outlineLevel="1">
+    <row r="430" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A430" s="5" t="s">
         <v>393</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="21" outlineLevel="1">
+    <row r="431" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A431" s="5" t="s">
         <v>393</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="21" outlineLevel="1">
+    <row r="432" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A432" s="5" t="s">
         <v>393</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21" outlineLevel="1">
+    <row r="433" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A433" s="5" t="s">
         <v>393</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21" outlineLevel="1">
+    <row r="434" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A434" s="5" t="s">
         <v>393</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21" outlineLevel="1">
+    <row r="435" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A435" s="5" t="s">
         <v>393</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21" outlineLevel="1">
+    <row r="436" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A436" s="5" t="s">
         <v>393</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21" outlineLevel="1">
+    <row r="437" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A437" s="5" t="s">
         <v>393</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="21" outlineLevel="1">
+    <row r="438" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A438" s="5" t="s">
         <v>393</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="21" outlineLevel="1">
+    <row r="439" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A439" s="5" t="s">
         <v>393</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21" outlineLevel="1">
+    <row r="440" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A440" s="5" t="s">
         <v>393</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="21" outlineLevel="1">
+    <row r="441" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A441" s="5" t="s">
         <v>393</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="21" outlineLevel="1">
+    <row r="442" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A442" s="5" t="s">
         <v>393</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21" outlineLevel="1">
+    <row r="443" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A443" s="5" t="s">
         <v>393</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21" outlineLevel="1">
+    <row r="444" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A444" s="5" t="s">
         <v>393</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21" outlineLevel="1">
+    <row r="445" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A445" s="5" t="s">
         <v>393</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21" outlineLevel="1">
+    <row r="446" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A446" s="5" t="s">
         <v>393</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:3" ht="21" outlineLevel="1">
+    <row r="447" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A447" s="5" t="s">
         <v>393</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="21" outlineLevel="1">
+    <row r="448" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A448" s="5" t="s">
         <v>393</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="21" outlineLevel="1">
+    <row r="449" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A449" s="5" t="s">
         <v>393</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="21" outlineLevel="1">
+    <row r="450" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A450" s="5" t="s">
         <v>393</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="21" outlineLevel="1">
+    <row r="451" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A451" s="5" t="s">
         <v>393</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="21" outlineLevel="1">
+    <row r="452" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A452" s="5" t="s">
         <v>393</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="21" outlineLevel="1">
+    <row r="453" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A453" s="5" t="s">
         <v>393</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="21" outlineLevel="1">
+    <row r="454" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A454" s="5" t="s">
         <v>393</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="21" outlineLevel="1">
+    <row r="455" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A455" s="5" t="s">
         <v>393</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="21" outlineLevel="1">
+    <row r="456" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A456" s="5" t="s">
         <v>393</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="21" outlineLevel="1">
+    <row r="457" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A457" s="5" t="s">
         <v>393</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="21" outlineLevel="1">
+    <row r="458" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A458" s="5" t="s">
         <v>393</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21" outlineLevel="1">
+    <row r="459" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A459" s="5" t="s">
         <v>393</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="21" outlineLevel="1">
+    <row r="460" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A460" s="5" t="s">
         <v>393</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:3" ht="21" outlineLevel="1">
+    <row r="461" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A461" s="5" t="s">
         <v>393</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="21" outlineLevel="1">
+    <row r="462" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A462" s="5" t="s">
         <v>393</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="21" outlineLevel="1">
+    <row r="463" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A463" s="5" t="s">
         <v>393</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21" outlineLevel="1">
+    <row r="464" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A464" s="5" t="s">
         <v>393</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="21" outlineLevel="1">
+    <row r="465" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A465" s="5" t="s">
         <v>393</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="21" outlineLevel="1">
+    <row r="466" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A466" s="5" t="s">
         <v>393</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="21" outlineLevel="1">
+    <row r="467" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A467" s="5" t="s">
         <v>393</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="21" outlineLevel="1">
+    <row r="468" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A468" s="5" t="s">
         <v>393</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:3" ht="21" outlineLevel="1">
+    <row r="469" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A469" s="5" t="s">
         <v>393</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="21" outlineLevel="1">
+    <row r="470" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A470" s="5" t="s">
         <v>393</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="471" spans="1:3" ht="21">
+    <row r="471" spans="1:3" ht="21" collapsed="1">
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>

</xml_diff>

<commit_message>
First Occurance And Last
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4AB2F8-026D-4C5D-B47D-7C8BBA850159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10279603-1B9E-435B-8F7E-79B956D3D7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="C362" sqref="C362"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3084,7 +3084,7 @@
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
     </row>
-    <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="102" spans="1:3" ht="21" outlineLevel="1">
       <c r="A102" s="5" t="s">
         <v>97</v>
       </c>
@@ -3092,10 +3092,10 @@
         <v>98</v>
       </c>
       <c r="C102" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="21" outlineLevel="1">
       <c r="A103" s="5" t="s">
         <v>97</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="104" spans="1:3" ht="21" outlineLevel="1">
       <c r="A104" s="5" t="s">
         <v>97</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="105" spans="1:3" ht="21" outlineLevel="1">
       <c r="A105" s="5" t="s">
         <v>97</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="106" spans="1:3" ht="21" outlineLevel="1">
       <c r="A106" s="5" t="s">
         <v>97</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="107" spans="1:3" ht="21" outlineLevel="1">
       <c r="A107" s="5" t="s">
         <v>97</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="108" spans="1:3" ht="21" outlineLevel="1">
       <c r="A108" s="5" t="s">
         <v>97</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="109" spans="1:3" ht="21" outlineLevel="1">
       <c r="A109" s="5" t="s">
         <v>97</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="110" spans="1:3" ht="21" outlineLevel="1">
       <c r="A110" s="5" t="s">
         <v>97</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="111" spans="1:3" ht="21" outlineLevel="1">
       <c r="A111" s="5" t="s">
         <v>97</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="112" spans="1:3" ht="21" outlineLevel="1">
       <c r="A112" s="5" t="s">
         <v>97</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="113" spans="1:3" ht="21" outlineLevel="1">
       <c r="A113" s="5" t="s">
         <v>97</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="114" spans="1:3" ht="21" outlineLevel="1">
       <c r="A114" s="5" t="s">
         <v>97</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="115" spans="1:3" ht="21" outlineLevel="1">
       <c r="A115" s="5" t="s">
         <v>97</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="116" spans="1:3" ht="21" outlineLevel="1">
       <c r="A116" s="5" t="s">
         <v>97</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="117" spans="1:3" ht="21" outlineLevel="1">
       <c r="A117" s="5" t="s">
         <v>97</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="118" spans="1:3" ht="21" outlineLevel="1">
       <c r="A118" s="5" t="s">
         <v>97</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="119" spans="1:3" ht="21" outlineLevel="1">
       <c r="A119" s="5" t="s">
         <v>97</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="120" spans="1:3" ht="21" outlineLevel="1">
       <c r="A120" s="5" t="s">
         <v>97</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="121" spans="1:3" ht="21" outlineLevel="1">
       <c r="A121" s="5" t="s">
         <v>97</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="122" spans="1:3" ht="21" outlineLevel="1">
       <c r="A122" s="5" t="s">
         <v>97</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="123" spans="1:3" ht="21" outlineLevel="1">
       <c r="A123" s="5" t="s">
         <v>97</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="124" spans="1:3" ht="21" outlineLevel="1">
       <c r="A124" s="5" t="s">
         <v>97</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="125" spans="1:3" ht="21" outlineLevel="1">
       <c r="A125" s="5" t="s">
         <v>97</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="126" spans="1:3" ht="21" outlineLevel="1">
       <c r="A126" s="5" t="s">
         <v>97</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="127" spans="1:3" ht="21" outlineLevel="1">
       <c r="A127" s="5" t="s">
         <v>97</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="128" spans="1:3" ht="21" outlineLevel="1">
       <c r="A128" s="5" t="s">
         <v>97</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="129" spans="1:3" ht="21" outlineLevel="1">
       <c r="A129" s="5" t="s">
         <v>97</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="130" spans="1:3" ht="21" outlineLevel="1">
       <c r="A130" s="5" t="s">
         <v>97</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="131" spans="1:3" ht="21" outlineLevel="1">
       <c r="A131" s="5" t="s">
         <v>97</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="132" spans="1:3" ht="21" outlineLevel="1">
       <c r="A132" s="5" t="s">
         <v>97</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="133" spans="1:3" ht="21" outlineLevel="1">
       <c r="A133" s="5" t="s">
         <v>97</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="134" spans="1:3" ht="21" outlineLevel="1">
       <c r="A134" s="5" t="s">
         <v>97</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="135" spans="1:3" ht="21" outlineLevel="1">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="136" spans="1:3" ht="21" outlineLevel="1">
       <c r="A136" s="5" t="s">
         <v>97</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="137" spans="1:3" ht="21" outlineLevel="1">
       <c r="A137" s="5" t="s">
         <v>97</v>
       </c>
@@ -3480,7 +3480,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
       <c r="A139" s="23" t="s">
         <v>134</v>
@@ -5794,7 +5793,7 @@
       <c r="B356" s="24"/>
       <c r="C356" s="24"/>
     </row>
-    <row r="357" spans="1:3" ht="21" outlineLevel="1">
+    <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
         <v>343</v>
       </c>
@@ -5805,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="21" outlineLevel="1">
+    <row r="358" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A358" s="8" t="s">
         <v>343</v>
       </c>
@@ -5816,7 +5815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="21" outlineLevel="1">
+    <row r="359" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A359" s="8" t="s">
         <v>343</v>
       </c>
@@ -5827,7 +5826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:3" ht="21" outlineLevel="1">
+    <row r="360" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A360" s="8" t="s">
         <v>343</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:3" ht="21" outlineLevel="1">
+    <row r="361" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A361" s="8" t="s">
         <v>343</v>
       </c>
@@ -5849,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:3" ht="21" outlineLevel="1">
+    <row r="362" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A362" s="8" t="s">
         <v>343</v>
       </c>
@@ -5860,7 +5859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:3" ht="21" outlineLevel="1">
+    <row r="363" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A363" s="8" t="s">
         <v>343</v>
       </c>
@@ -5871,7 +5870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:3" ht="21" outlineLevel="1">
+    <row r="364" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A364" s="8" t="s">
         <v>343</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:3" ht="21" outlineLevel="1">
+    <row r="365" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A365" s="8" t="s">
         <v>343</v>
       </c>
@@ -5893,7 +5892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:3" ht="21" outlineLevel="1">
+    <row r="366" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A366" s="8" t="s">
         <v>343</v>
       </c>
@@ -5904,7 +5903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:3" ht="21" outlineLevel="1">
+    <row r="367" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A367" s="8" t="s">
         <v>343</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:3" ht="21" outlineLevel="1">
+    <row r="368" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A368" s="8" t="s">
         <v>343</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:3" ht="21" outlineLevel="1">
+    <row r="369" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A369" s="8" t="s">
         <v>343</v>
       </c>
@@ -5937,7 +5936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:3" ht="21" outlineLevel="1">
+    <row r="370" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A370" s="8" t="s">
         <v>343</v>
       </c>
@@ -5948,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:3" ht="21" outlineLevel="1">
+    <row r="371" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A371" s="8" t="s">
         <v>343</v>
       </c>
@@ -5959,7 +5958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:3" ht="21" outlineLevel="1">
+    <row r="372" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A372" s="8" t="s">
         <v>343</v>
       </c>
@@ -5970,7 +5969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:3" ht="21" outlineLevel="1">
+    <row r="373" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A373" s="8" t="s">
         <v>343</v>
       </c>
@@ -5981,7 +5980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:3" ht="21" outlineLevel="1">
+    <row r="374" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A374" s="8" t="s">
         <v>343</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:3" ht="21" outlineLevel="1">
+    <row r="375" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A375" s="8" t="s">
         <v>343</v>
       </c>
@@ -6003,7 +6002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:3" ht="21" outlineLevel="1">
+    <row r="376" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A376" s="8" t="s">
         <v>343</v>
       </c>
@@ -6014,7 +6013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:3" ht="21" outlineLevel="1">
+    <row r="377" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A377" s="8" t="s">
         <v>343</v>
       </c>
@@ -6025,7 +6024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:3" ht="21" outlineLevel="1">
+    <row r="378" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A378" s="8" t="s">
         <v>343</v>
       </c>
@@ -6036,7 +6035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:3" ht="21" outlineLevel="1">
+    <row r="379" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A379" s="8" t="s">
         <v>343</v>
       </c>
@@ -6047,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:3" ht="21" outlineLevel="1">
+    <row r="380" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A380" s="8" t="s">
         <v>343</v>
       </c>
@@ -6058,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:3" ht="21" outlineLevel="1">
+    <row r="381" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A381" s="8" t="s">
         <v>343</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:3" ht="21" outlineLevel="1">
+    <row r="382" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A382" s="8" t="s">
         <v>343</v>
       </c>
@@ -6080,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:3" ht="21" outlineLevel="1">
+    <row r="383" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A383" s="8" t="s">
         <v>343</v>
       </c>
@@ -6091,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:3" ht="21" outlineLevel="1">
+    <row r="384" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A384" s="8" t="s">
         <v>343</v>
       </c>
@@ -6102,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="21" outlineLevel="1">
+    <row r="385" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A385" s="8" t="s">
         <v>343</v>
       </c>
@@ -6113,7 +6112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="21" outlineLevel="1">
+    <row r="386" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A386" s="8" t="s">
         <v>343</v>
       </c>
@@ -6124,7 +6123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="21" outlineLevel="1">
+    <row r="387" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A387" s="8" t="s">
         <v>343</v>
       </c>
@@ -6135,7 +6134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="21" outlineLevel="1">
+    <row r="388" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A388" s="8" t="s">
         <v>343</v>
       </c>
@@ -6146,7 +6145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="21" outlineLevel="1">
+    <row r="389" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A389" s="8" t="s">
         <v>343</v>
       </c>
@@ -6157,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="21" outlineLevel="1">
+    <row r="390" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A390" s="8" t="s">
         <v>343</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="21" outlineLevel="1">
+    <row r="391" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A391" s="8" t="s">
         <v>343</v>
       </c>
@@ -6179,7 +6178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="21" outlineLevel="1">
+    <row r="392" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A392" s="8" t="s">
         <v>343</v>
       </c>
@@ -6190,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="21" outlineLevel="1">
+    <row r="393" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A393" s="8" t="s">
         <v>343</v>
       </c>
@@ -6201,7 +6200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="21" outlineLevel="1">
+    <row r="394" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A394" s="8" t="s">
         <v>343</v>
       </c>
@@ -6212,7 +6211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="21" outlineLevel="1">
+    <row r="395" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A395" s="8" t="s">
         <v>343</v>
       </c>
@@ -6223,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="21" outlineLevel="1">
+    <row r="396" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A396" s="8" t="s">
         <v>343</v>
       </c>
@@ -6234,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="21" outlineLevel="1">
+    <row r="397" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A397" s="8" t="s">
         <v>343</v>
       </c>
@@ -6245,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="21" outlineLevel="1">
+    <row r="398" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A398" s="8" t="s">
         <v>343</v>
       </c>
@@ -6256,7 +6255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:3" ht="21" outlineLevel="1">
+    <row r="399" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A399" s="8" t="s">
         <v>343</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="21" outlineLevel="1">
+    <row r="400" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A400" s="8" t="s">
         <v>343</v>
       </c>
@@ -6278,7 +6277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="21">
+    <row r="401" spans="1:3" ht="21" collapsed="1">
       <c r="B401" s="7"/>
       <c r="C401" s="4"/>
     </row>
@@ -7623,7 +7622,7 @@
   <dimension ref="B2:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -7656,7 +7655,9 @@
       <c r="C4" s="17">
         <v>10</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="17">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="18">

</xml_diff>

<commit_message>
Search In Rotated Sorted Array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10279603-1B9E-435B-8F7E-79B956D3D7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9260F59-ABB8-4C72-A40B-E0256CAA9D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1673,7 +1673,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1685,16 +1694,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2065,15 +2065,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2479,11 +2479,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3078,11 +3078,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3114,7 +3114,7 @@
         <v>100</v>
       </c>
       <c r="C104" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21" outlineLevel="1">
@@ -3481,11 +3481,11 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3883,11 +3883,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4280,11 +4280,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4533,11 +4533,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4929,11 +4929,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5149,11 +5149,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5578,11 +5578,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5787,11 +5787,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6282,11 +6282,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6359,11 +6359,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7030,11 +7030,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7149,21 +7149,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Implement Queue from Scratch
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD31905-265A-4455-9937-E8BFC27EBE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E920B4F-B89F-45F6-965E-35D21B1510B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1673,7 +1673,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1685,16 +1694,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2018,7 +2018,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C297" sqref="C297"/>
+      <selection activeCell="C301" sqref="C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2065,15 +2065,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2479,11 +2479,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3078,11 +3078,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3482,11 +3482,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3884,11 +3884,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4281,11 +4281,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4534,11 +4534,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4930,11 +4930,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5150,11 +5150,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5175,7 +5175,7 @@
         <v>287</v>
       </c>
       <c r="C298" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21" outlineLevel="1">
@@ -5579,11 +5579,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5788,11 +5788,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6283,11 +6283,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6360,11 +6360,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7031,11 +7031,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7150,21 +7150,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximum Sum Increasing Subsequence
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21719305-ED55-4D1C-A322-2A6AA41DD072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D774CC1C-BBB7-451F-9925-1FEC8DA77F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="C429" sqref="C429"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="C430" sqref="C430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6569,7 +6569,7 @@
         <v>410</v>
       </c>
       <c r="C429" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Longest subsequence such that difference between adjacent is one
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7E8D6F-0BE5-4940-BA89-48B191DD97C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5317927-F6AB-4F13-B901-0C2EC75470C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B426" workbookViewId="0">
-      <selection activeCell="C431" sqref="C431"/>
+      <selection activeCell="C433" sqref="C433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6591,7 +6591,7 @@
         <v>412</v>
       </c>
       <c r="C431" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Pairs With Certain Difference
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578393DF-DC52-420C-9212-FC61026D8985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7079FFC3-14BD-40CF-A00A-E3457590C5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B426" workbookViewId="0">
-      <selection activeCell="C433" sqref="C433"/>
+    <sheetView tabSelected="1" topLeftCell="B427" workbookViewId="0">
+      <selection activeCell="C437" sqref="C437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6646,7 +6646,7 @@
         <v>417</v>
       </c>
       <c r="C436" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
maximum difference between the number of 0s and the number of 1s
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5901C976-0D42-44AF-A665-0F8594BF2DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96812A7-DA30-461A-A3F0-F72A066FCEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B425" workbookViewId="0">
-      <selection activeCell="C438" sqref="C438"/>
+    <sheetView tabSelected="1" topLeftCell="B424" workbookViewId="0">
+      <selection activeCell="C439" sqref="C439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6668,7 +6668,7 @@
         <v>419</v>
       </c>
       <c r="C438" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="439" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Minimum Number Of Jumps To Reach End
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96812A7-DA30-461A-A3F0-F72A066FCEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39DFECC-A669-4106-B837-EFD22E68BFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B424" workbookViewId="0">
-      <selection activeCell="C439" sqref="C439"/>
+      <selection activeCell="C440" sqref="C440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6679,7 +6679,7 @@
         <v>420</v>
       </c>
       <c r="C439" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Minimum Cost to Fill Given Weight In a Bag
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39DFECC-A669-4106-B837-EFD22E68BFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51A966C-0B9F-4C02-ADF9-3BF3638D0A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B424" workbookViewId="0">
-      <selection activeCell="C440" sqref="C440"/>
+    <sheetView tabSelected="1" topLeftCell="C424" workbookViewId="0">
+      <selection activeCell="C441" sqref="C441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6690,7 +6690,7 @@
         <v>421</v>
       </c>
       <c r="C440" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Minimum removals from array to make max – min less than or equal to K
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51A966C-0B9F-4C02-ADF9-3BF3638D0A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9405CBBF-21EC-4060-A553-DB7757695512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C424" workbookViewId="0">
-      <selection activeCell="C441" sqref="C441"/>
+    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
+      <selection activeCell="B441" sqref="B441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6701,7 +6701,7 @@
         <v>422</v>
       </c>
       <c r="C441" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Reach a Given Score
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE224DCD-88A2-42C2-93A1-7395B8983CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7044653-7E82-49C5-A9D7-31637D9300CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B425" workbookViewId="0">
-      <selection activeCell="C443" sqref="C443"/>
+    <sheetView tabSelected="1" topLeftCell="B432" workbookViewId="0">
+      <selection activeCell="C444" sqref="C444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6723,7 +6723,7 @@
         <v>424</v>
       </c>
       <c r="C443" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Count Balanced Binary Trees of Height h
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7044653-7E82-49C5-A9D7-31637D9300CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6EF6CC-A13A-40E5-BFC8-3D9559EAD0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,7 +2014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B432" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A427" workbookViewId="0">
       <selection activeCell="C444" sqref="C444"/>
     </sheetView>
   </sheetViews>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6734,7 +6734,7 @@
         <v>425</v>
       </c>
       <c r="C444" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Smallest Sum Contiguous Subarray
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA071D3-B7C7-4322-9E0B-DE04FA46F3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A0DE27-CFA1-4300-AF13-EA56305BEE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" workbookViewId="0">
-      <selection activeCell="C446" sqref="C446"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="C447" sqref="C447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6756,7 +6756,7 @@
         <v>427</v>
       </c>
       <c r="C446" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="447" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Largest Independent Set Problem
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E7D60-FAD4-4432-B80C-BDFA43495EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4309CBD-41F3-48F2-B9B1-2D40AEA8B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A441" workbookViewId="0">
-      <selection activeCell="C448" sqref="C448"/>
+      <selection activeCell="C450" sqref="C450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6789,7 +6789,7 @@
         <v>430</v>
       </c>
       <c r="C449" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximum profit by buying and selling a share at most twice
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22737D48-9364-4646-BA8B-5C0BCE8A0BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD1C77-1821-40D1-9778-8109C12CB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C458" sqref="C458"/>
+      <selection activeCell="C459" sqref="C459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6888,7 +6888,7 @@
         <v>439</v>
       </c>
       <c r="C458" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Optimal Strategy For A Game
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD1C77-1821-40D1-9778-8109C12CB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD0246-76FD-4691-9759-681D2459B549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C459" sqref="C459"/>
+      <selection activeCell="C460" sqref="C460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3075,11 +3075,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3479,11 +3479,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3881,11 +3881,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4278,11 +4278,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4531,11 +4531,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4927,11 +4927,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5147,11 +5147,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5576,11 +5576,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5785,11 +5785,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6280,11 +6280,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6357,11 +6357,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6899,7 +6899,7 @@
         <v>440</v>
       </c>
       <c r="C459" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="460" spans="1:3" ht="21" outlineLevel="1">
@@ -7028,11 +7028,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7147,21 +7147,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Largest Rectangular Sub-matrix whose sum is 0
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7198C59-EFB3-4029-BD80-E6590609BF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716475D9-8E26-46B8-8CFB-449E9E204798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1670,7 +1670,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1682,16 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C464" sqref="C464"/>
+      <selection activeCell="C466" sqref="C466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="23" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
     </row>
     <row r="57" spans="1:3" ht="21" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3074,11 +3074,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3478,11 +3478,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3880,11 +3880,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+      <c r="A177" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4277,11 +4277,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+      <c r="A214" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
+      <c r="B214" s="23"/>
+      <c r="C214" s="23"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4530,11 +4530,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+      <c r="A238" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4926,11 +4926,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="23"/>
+      <c r="C275" s="23"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5146,11 +5146,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5575,11 +5575,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="23"/>
+      <c r="C336" s="23"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5784,11 +5784,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+      <c r="A356" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
+      <c r="B356" s="19"/>
+      <c r="C356" s="19"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6279,11 +6279,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="20"/>
+      <c r="C402" s="20"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6356,11 +6356,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="21"/>
+      <c r="C410" s="21"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6952,8 +6952,8 @@
       <c r="B464" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="C464" s="4" t="b">
-        <v>0</v>
+      <c r="C464" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="465" spans="1:3" ht="21" outlineLevel="1">
@@ -6964,7 +6964,7 @@
         <v>446</v>
       </c>
       <c r="C465" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="466" spans="1:3" ht="21" outlineLevel="1">
@@ -7027,11 +7027,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="22"/>
+      <c r="C472" s="22"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7146,21 +7146,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Largest area rectangular sub-matrix with equal number of 1’s and 0’s
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716475D9-8E26-46B8-8CFB-449E9E204798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A58DC9-44FD-435B-B50A-F709A848A554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1670,16 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,7 +1682,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C466" sqref="C466"/>
+      <selection activeCell="A462" sqref="A462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2062,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2476,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,11 +2594,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3" ht="21" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3074,11 +3074,11 @@
       </c>
     </row>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3478,11 +3478,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="22" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3880,11 +3880,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="26"/>
-      <c r="C177" s="26"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4277,11 +4277,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="23" t="s">
+      <c r="A214" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="23"/>
-      <c r="C214" s="23"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="20"/>
     </row>
     <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4530,11 +4530,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="26"/>
-      <c r="C238" s="26"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="19"/>
     </row>
     <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4926,11 +4926,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="23" t="s">
+      <c r="A275" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="23"/>
-      <c r="C275" s="23"/>
+      <c r="B275" s="20"/>
+      <c r="C275" s="20"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5146,11 +5146,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="26"/>
-      <c r="C296" s="26"/>
+      <c r="B296" s="19"/>
+      <c r="C296" s="19"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5575,11 +5575,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="23" t="s">
+      <c r="A336" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="23"/>
-      <c r="C336" s="23"/>
+      <c r="B336" s="20"/>
+      <c r="C336" s="20"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5784,11 +5784,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="19" t="s">
+      <c r="A356" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="19"/>
-      <c r="C356" s="19"/>
+      <c r="B356" s="24"/>
+      <c r="C356" s="24"/>
     </row>
     <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6279,11 +6279,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="20" t="s">
+      <c r="A402" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="20"/>
-      <c r="C402" s="20"/>
+      <c r="B402" s="25"/>
+      <c r="C402" s="25"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6356,11 +6356,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="21" t="s">
+      <c r="A410" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="21"/>
+      <c r="B410" s="26"/>
+      <c r="C410" s="26"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6975,7 +6975,7 @@
         <v>447</v>
       </c>
       <c r="C466" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="467" spans="1:3" ht="21" outlineLevel="1">
@@ -7027,11 +7027,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="22" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="22"/>
-      <c r="C472" s="22"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7146,21 +7146,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximum Sum Rectangle in 2D Matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A58DC9-44FD-435B-B50A-F709A848A554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0755CA-5067-4CCE-BFD2-979187AAB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1482,7 +1482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1573,6 +1573,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1634,7 +1641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1670,6 +1677,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2014,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="A462" sqref="A462"/>
+    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
+      <selection activeCell="A458" sqref="A458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2050,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>252</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2062,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2476,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2594,13 +2604,13 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-    </row>
-    <row r="57" spans="1:3" ht="21" outlineLevel="1">
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+    </row>
+    <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" outlineLevel="1">
+    <row r="58" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A58" s="5" t="s">
         <v>53</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21" outlineLevel="1">
+    <row r="59" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
@@ -2633,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21" outlineLevel="1">
+    <row r="60" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
@@ -2644,7 +2654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21" outlineLevel="1">
+    <row r="61" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A61" s="5" t="s">
         <v>53</v>
       </c>
@@ -2655,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21" outlineLevel="1">
+    <row r="62" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A62" s="5" t="s">
         <v>53</v>
       </c>
@@ -2666,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21" outlineLevel="1">
+    <row r="63" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A63" s="5" t="s">
         <v>53</v>
       </c>
@@ -2677,7 +2687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" outlineLevel="1">
+    <row r="64" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A64" s="5" t="s">
         <v>53</v>
       </c>
@@ -2688,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21" outlineLevel="1">
+    <row r="65" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A65" s="5" t="s">
         <v>53</v>
       </c>
@@ -2699,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="21" outlineLevel="1">
+    <row r="66" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A66" s="5" t="s">
         <v>53</v>
       </c>
@@ -2710,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21" outlineLevel="1">
+    <row r="67" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A67" s="5" t="s">
         <v>53</v>
       </c>
@@ -2721,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21" outlineLevel="1">
+    <row r="68" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
@@ -2732,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="21" outlineLevel="1">
+    <row r="69" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A69" s="5" t="s">
         <v>53</v>
       </c>
@@ -2743,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="21" outlineLevel="1">
+    <row r="70" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="21" outlineLevel="1">
+    <row r="71" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A71" s="5" t="s">
         <v>53</v>
       </c>
@@ -2765,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="21" outlineLevel="1">
+    <row r="72" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
@@ -2776,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="21" outlineLevel="1">
+    <row r="73" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="21" outlineLevel="1">
+    <row r="74" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A74" s="5" t="s">
         <v>53</v>
       </c>
@@ -2798,7 +2808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="21" outlineLevel="1">
+    <row r="75" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A75" s="5" t="s">
         <v>53</v>
       </c>
@@ -2809,7 +2819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21" outlineLevel="1">
+    <row r="76" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
@@ -2820,7 +2830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="21" outlineLevel="1">
+    <row r="77" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A77" s="5" t="s">
         <v>53</v>
       </c>
@@ -2831,7 +2841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="21" outlineLevel="1">
+    <row r="78" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A78" s="5" t="s">
         <v>53</v>
       </c>
@@ -2842,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="21" outlineLevel="1">
+    <row r="79" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A79" s="5" t="s">
         <v>53</v>
       </c>
@@ -2853,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="21" outlineLevel="1">
+    <row r="80" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A80" s="5" t="s">
         <v>53</v>
       </c>
@@ -2864,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="21" outlineLevel="1">
+    <row r="81" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -2875,7 +2885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="21" outlineLevel="1">
+    <row r="82" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A82" s="5" t="s">
         <v>53</v>
       </c>
@@ -2886,7 +2896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="21" outlineLevel="1">
+    <row r="83" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A83" s="5" t="s">
         <v>53</v>
       </c>
@@ -2897,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="21" outlineLevel="1">
+    <row r="84" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A84" s="5" t="s">
         <v>53</v>
       </c>
@@ -2908,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="21" outlineLevel="1">
+    <row r="85" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A85" s="5" t="s">
         <v>53</v>
       </c>
@@ -2919,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="21" outlineLevel="1">
+    <row r="86" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A86" s="5" t="s">
         <v>53</v>
       </c>
@@ -2930,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="21" outlineLevel="1">
+    <row r="87" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A87" s="5" t="s">
         <v>53</v>
       </c>
@@ -2941,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="21" outlineLevel="1">
+    <row r="88" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A88" s="5" t="s">
         <v>53</v>
       </c>
@@ -2952,7 +2962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="21" outlineLevel="1">
+    <row r="89" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A89" s="5" t="s">
         <v>53</v>
       </c>
@@ -2963,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="21" outlineLevel="1">
+    <row r="90" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A90" s="5" t="s">
         <v>53</v>
       </c>
@@ -2974,7 +2984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="21" outlineLevel="1">
+    <row r="91" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A91" s="5" t="s">
         <v>53</v>
       </c>
@@ -2985,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="21" outlineLevel="1">
+    <row r="92" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A92" s="5" t="s">
         <v>53</v>
       </c>
@@ -2996,7 +3006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="21" outlineLevel="1">
+    <row r="93" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A93" s="5" t="s">
         <v>53</v>
       </c>
@@ -3007,7 +3017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="21" outlineLevel="1">
+    <row r="94" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A94" s="5" t="s">
         <v>53</v>
       </c>
@@ -3018,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="21" outlineLevel="1">
+    <row r="95" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A95" s="5" t="s">
         <v>53</v>
       </c>
@@ -3029,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="21" outlineLevel="1">
+    <row r="96" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A96" s="5" t="s">
         <v>53</v>
       </c>
@@ -3040,7 +3050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21" outlineLevel="1">
+    <row r="97" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A97" s="5" t="s">
         <v>53</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="21" outlineLevel="1">
+    <row r="98" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A98" s="5" t="s">
         <v>53</v>
       </c>
@@ -3062,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="21" outlineLevel="1">
+    <row r="99" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A99" s="5" t="s">
         <v>53</v>
       </c>
@@ -3073,12 +3083,13 @@
         <v>4</v>
       </c>
     </row>
+    <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3478,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3879,14 +3890,14 @@
       <c r="C175" s="4"/>
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
-    <row r="177" spans="1:3" ht="21">
-      <c r="A177" s="19" t="s">
+    <row r="177" spans="1:4" ht="21">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="19"/>
-      <c r="C177" s="19"/>
-    </row>
-    <row r="178" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
+    </row>
+    <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
@@ -3896,8 +3907,11 @@
       <c r="C178" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D178" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
@@ -3907,8 +3921,11 @@
       <c r="C179" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D179" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
@@ -3918,8 +3935,11 @@
       <c r="C180" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D180" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
@@ -3929,8 +3949,11 @@
       <c r="C181" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D181" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
@@ -3940,8 +3963,11 @@
       <c r="C182" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D182" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
@@ -3951,8 +3977,11 @@
       <c r="C183" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D183" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
@@ -3962,8 +3991,11 @@
       <c r="C184" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D184" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
@@ -3973,8 +4005,11 @@
       <c r="C185" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D185" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
@@ -3984,8 +4019,11 @@
       <c r="C186" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D186" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
@@ -3995,8 +4033,11 @@
       <c r="C187" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D187" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
@@ -4006,8 +4047,11 @@
       <c r="C188" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D188" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
@@ -4017,8 +4061,11 @@
       <c r="C189" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D189" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
@@ -4028,8 +4075,11 @@
       <c r="C190" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D190" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
@@ -4039,8 +4089,11 @@
       <c r="C191" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D191" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
@@ -4050,8 +4103,11 @@
       <c r="C192" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D192" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -4061,30 +4117,39 @@
       <c r="C193" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D193" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C194" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C194" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C195" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C195" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D195" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -4094,41 +4159,53 @@
       <c r="C196" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D196" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C197" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C197" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D197" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C198" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C198" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D198" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B199" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C199" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C199" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D199" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -4138,19 +4215,25 @@
       <c r="C200" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D200" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C201" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C201" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D201" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
@@ -4160,19 +4243,25 @@
       <c r="C202" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D202" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C203" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C203" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
@@ -4182,19 +4271,25 @@
       <c r="C204" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D204" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C205" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C205" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D205" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
@@ -4204,63 +4299,81 @@
       <c r="C206" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D206" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C207" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C207" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D207" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C208" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C208" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D208" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A209" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B209" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C209" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C209" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D209" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A210" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B210" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C210" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C210" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D210" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A211" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B211" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C211" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C211" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D211" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A212" s="5" t="s">
         <v>171</v>
       </c>
@@ -4270,20 +4383,23 @@
       <c r="C212" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" ht="21" collapsed="1">
+      <c r="D212" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="21" collapsed="1">
       <c r="A213" s="8"/>
       <c r="B213" s="7"/>
       <c r="C213" s="4"/>
     </row>
-    <row r="214" spans="1:3" ht="21">
-      <c r="A214" s="20" t="s">
+    <row r="214" spans="1:4" ht="21">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="20"/>
-      <c r="C214" s="20"/>
-    </row>
-    <row r="215" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
+    </row>
+    <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
         <v>207</v>
       </c>
@@ -4293,8 +4409,11 @@
       <c r="C215" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D215" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A216" s="5" t="s">
         <v>207</v>
       </c>
@@ -4304,41 +4423,53 @@
       <c r="C216" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D216" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A217" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B217" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C217" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C217" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D217" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A218" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C218" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C218" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D218" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A219" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C219" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C219" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D219" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A220" s="5" t="s">
         <v>207</v>
       </c>
@@ -4348,96 +4479,123 @@
       <c r="C220" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D220" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A221" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B221" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C221" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C221" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D221" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A222" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C222" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C222" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D222" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A223" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C223" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C223" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D223" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A224" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C224" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C224" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D224" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A225" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C225" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C225" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D225" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A226" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C226" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C226" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D226" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A227" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C227" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C227" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D227" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A228" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C228" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C228" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D228" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A229" s="5" t="s">
         <v>207</v>
       </c>
@@ -4447,8 +4605,11 @@
       <c r="C229" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D229" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A230" s="5" t="s">
         <v>207</v>
       </c>
@@ -4458,85 +4619,106 @@
       <c r="C230" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D230" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A231" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B231" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C231" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C231" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D231" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A232" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B232" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C232" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A233" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C233" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C233" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D233" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A234" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B234" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C234" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C234" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D234" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A235" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B235" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C235" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C235" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D235" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A236" s="5" t="s">
         <v>207</v>
       </c>
       <c r="B236" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C236" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="21" collapsed="1">
+      <c r="C236" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D236" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="21" collapsed="1">
       <c r="B237" s="7"/>
       <c r="C237" s="4"/>
     </row>
-    <row r="238" spans="1:3" ht="21">
-      <c r="A238" s="19" t="s">
+    <row r="238" spans="1:4" ht="21">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="19"/>
-      <c r="C238" s="19"/>
-    </row>
-    <row r="239" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
+    </row>
+    <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
         <v>229</v>
       </c>
@@ -4547,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="240" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A240" s="5" t="s">
         <v>229</v>
       </c>
@@ -4926,11 +5108,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="20" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="20"/>
-      <c r="C275" s="20"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5146,11 +5328,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="19" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="19"/>
-      <c r="C296" s="19"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5575,11 +5757,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="20" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="20"/>
-      <c r="C336" s="20"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5757,7 +5939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="353" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A353" s="8" t="s">
         <v>323</v>
       </c>
@@ -5768,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="354" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A354" s="8" t="s">
         <v>323</v>
       </c>
@@ -5779,18 +5961,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:3" ht="21" collapsed="1">
+    <row r="355" spans="1:4" ht="21" collapsed="1">
       <c r="B355" s="7"/>
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="1:3" ht="21" customHeight="1">
-      <c r="A356" s="24" t="s">
+    <row r="356" spans="1:4" ht="21" customHeight="1">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="24"/>
-      <c r="C356" s="24"/>
-    </row>
-    <row r="357" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
+    </row>
+    <row r="357" spans="1:4" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
         <v>342</v>
       </c>
@@ -5801,7 +5983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="358" spans="1:4" ht="21" outlineLevel="1">
       <c r="A358" s="8" t="s">
         <v>342</v>
       </c>
@@ -5812,7 +5994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="359" spans="1:4" ht="21" outlineLevel="1">
       <c r="A359" s="8" t="s">
         <v>342</v>
       </c>
@@ -5823,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+    <row r="360" spans="1:4" ht="21" outlineLevel="1">
       <c r="A360" s="8" t="s">
         <v>342</v>
       </c>
@@ -5831,10 +6013,13 @@
         <v>346</v>
       </c>
       <c r="C360" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="361" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+        <v>1</v>
+      </c>
+      <c r="D360" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" ht="21" outlineLevel="1">
       <c r="A361" s="8" t="s">
         <v>342</v>
       </c>
@@ -5844,30 +6029,39 @@
       <c r="C361" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D361" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" ht="21" outlineLevel="1">
       <c r="A362" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B362" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C362" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="363" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C362" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D362" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" ht="21" outlineLevel="1">
       <c r="A363" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B363" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="C363" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="364" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C363" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D363" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" ht="21" outlineLevel="1">
       <c r="A364" s="8" t="s">
         <v>342</v>
       </c>
@@ -5877,8 +6071,11 @@
       <c r="C364" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D364" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" ht="21" outlineLevel="1">
       <c r="A365" s="8" t="s">
         <v>342</v>
       </c>
@@ -5888,30 +6085,39 @@
       <c r="C365" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="366" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D365" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" ht="21" outlineLevel="1">
       <c r="A366" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B366" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C366" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="367" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C366" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D366" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" ht="21" outlineLevel="1">
       <c r="A367" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B367" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C367" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="368" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C367" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D367" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" ht="21" outlineLevel="1">
       <c r="A368" s="8" t="s">
         <v>342</v>
       </c>
@@ -5921,8 +6127,11 @@
       <c r="C368" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D368" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" ht="21" outlineLevel="1">
       <c r="A369" s="8" t="s">
         <v>342</v>
       </c>
@@ -5932,19 +6141,25 @@
       <c r="C369" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D369" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" ht="21" outlineLevel="1">
       <c r="A370" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B370" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C370" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="371" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C370" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D370" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" ht="21" outlineLevel="1">
       <c r="A371" s="8" t="s">
         <v>342</v>
       </c>
@@ -5954,8 +6169,11 @@
       <c r="C371" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D371" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" ht="21" outlineLevel="1">
       <c r="A372" s="8" t="s">
         <v>342</v>
       </c>
@@ -5965,8 +6183,11 @@
       <c r="C372" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D372" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" ht="21" outlineLevel="1">
       <c r="A373" s="8" t="s">
         <v>342</v>
       </c>
@@ -5976,8 +6197,11 @@
       <c r="C373" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D373" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" ht="21" outlineLevel="1">
       <c r="A374" s="8" t="s">
         <v>342</v>
       </c>
@@ -5987,8 +6211,11 @@
       <c r="C374" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D374" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" ht="21" outlineLevel="1">
       <c r="A375" s="8" t="s">
         <v>342</v>
       </c>
@@ -5998,8 +6225,11 @@
       <c r="C375" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D375" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" ht="21" outlineLevel="1">
       <c r="A376" s="8" t="s">
         <v>342</v>
       </c>
@@ -6009,8 +6239,11 @@
       <c r="C376" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D376" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" ht="21" outlineLevel="1">
       <c r="A377" s="8" t="s">
         <v>342</v>
       </c>
@@ -6020,8 +6253,11 @@
       <c r="C377" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D377" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" ht="21" outlineLevel="1">
       <c r="A378" s="8" t="s">
         <v>342</v>
       </c>
@@ -6031,8 +6267,11 @@
       <c r="C378" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D378" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" ht="21" outlineLevel="1">
       <c r="A379" s="8" t="s">
         <v>342</v>
       </c>
@@ -6042,8 +6281,11 @@
       <c r="C379" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="380" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D379" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" ht="21" outlineLevel="1">
       <c r="A380" s="8" t="s">
         <v>342</v>
       </c>
@@ -6053,19 +6295,25 @@
       <c r="C380" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="381" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D380" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" ht="21" outlineLevel="1">
       <c r="A381" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B381" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C381" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C381" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D381" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" ht="21" outlineLevel="1">
       <c r="A382" s="8" t="s">
         <v>342</v>
       </c>
@@ -6075,8 +6323,11 @@
       <c r="C382" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="383" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D382" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" ht="21" outlineLevel="1">
       <c r="A383" s="8" t="s">
         <v>342</v>
       </c>
@@ -6086,8 +6337,11 @@
       <c r="C383" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="384" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D383" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" ht="21" outlineLevel="1">
       <c r="A384" s="8" t="s">
         <v>342</v>
       </c>
@@ -6097,8 +6351,11 @@
       <c r="C384" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="385" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D384" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" ht="21" outlineLevel="1">
       <c r="A385" s="8" t="s">
         <v>342</v>
       </c>
@@ -6108,19 +6365,25 @@
       <c r="C385" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D385" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" ht="21" outlineLevel="1">
       <c r="A386" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B386" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C386" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="387" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C386" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D386" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" ht="21" outlineLevel="1">
       <c r="A387" s="8" t="s">
         <v>342</v>
       </c>
@@ -6130,118 +6393,151 @@
       <c r="C387" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D387" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" ht="21" outlineLevel="1">
       <c r="A388" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B388" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="C388" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="389" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C388" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D388" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" ht="21" outlineLevel="1">
       <c r="A389" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B389" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="C389" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="390" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C389" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D389" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" ht="21" outlineLevel="1">
       <c r="A390" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B390" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="C390" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="391" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C390" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D390" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" ht="21" outlineLevel="1">
       <c r="A391" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B391" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="C391" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="392" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C391" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D391" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" ht="21" outlineLevel="1">
       <c r="A392" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B392" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="C392" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="393" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C392" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D392" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" ht="21" outlineLevel="1">
       <c r="A393" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B393" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C393" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="394" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C393" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D393" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" ht="21" outlineLevel="1">
       <c r="A394" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B394" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="C394" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="395" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C394" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D394" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" ht="21" outlineLevel="1">
       <c r="A395" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B395" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="C395" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="396" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C395" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D395" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" ht="21" outlineLevel="1">
       <c r="A396" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B396" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="C396" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="397" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C396" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D396" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" ht="21" outlineLevel="1">
       <c r="A397" s="8" t="s">
         <v>342</v>
       </c>
       <c r="B397" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="C397" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="398" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="C397" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D397" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" ht="21" outlineLevel="1">
       <c r="A398" s="8" t="s">
         <v>342</v>
       </c>
@@ -6251,8 +6547,11 @@
       <c r="C398" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D398" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" ht="21" outlineLevel="1">
       <c r="A399" s="8" t="s">
         <v>342</v>
       </c>
@@ -6262,8 +6561,11 @@
       <c r="C399" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="400" spans="1:3" ht="21" hidden="1" outlineLevel="1">
+      <c r="D399" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" ht="21" outlineLevel="1">
       <c r="A400" s="8" t="s">
         <v>342</v>
       </c>
@@ -6273,17 +6575,20 @@
       <c r="C400" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="401" spans="1:3" ht="21" collapsed="1">
+      <c r="D400" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" ht="21">
       <c r="B401" s="7"/>
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="25" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="25"/>
-      <c r="C402" s="25"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6356,11 +6661,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="26"/>
-      <c r="C410" s="26"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -6986,7 +7291,7 @@
         <v>448</v>
       </c>
       <c r="C467" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468" spans="1:3" ht="21" outlineLevel="1">
@@ -6996,8 +7301,8 @@
       <c r="B468" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="C468" s="4" t="b">
-        <v>0</v>
+      <c r="C468" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="469" spans="1:3" ht="21" outlineLevel="1">
@@ -7027,11 +7332,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7628,11 +7933,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" s="17" t="s">

</xml_diff>

<commit_message>
Detect Cycle in UnDirected Graph using BFS/DFS Algo
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0755CA-5067-4CCE-BFD2-979187AAB1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3939A867-4209-455F-94C4-615F97E44A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="A458" sqref="A458"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="C362" sqref="C362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3891,11 +3891,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4393,11 +4393,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4712,11 +4712,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5108,11 +5108,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5328,11 +5328,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5757,11 +5757,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5966,11 +5966,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6027,7 +6027,7 @@
         <v>347</v>
       </c>
       <c r="C361" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D361" s="4" t="b">
         <v>0</v>
@@ -6584,11 +6584,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6661,13 +6661,13 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
-    </row>
-    <row r="411" spans="1:3" ht="21" outlineLevel="1">
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
+    </row>
+    <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
         <v>392</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="21" outlineLevel="1">
+    <row r="412" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A412" s="5" t="s">
         <v>392</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="21" outlineLevel="1">
+    <row r="413" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A413" s="5" t="s">
         <v>392</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="21" outlineLevel="1">
+    <row r="414" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A414" s="5" t="s">
         <v>392</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:3" ht="21" outlineLevel="1">
+    <row r="415" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A415" s="5" t="s">
         <v>392</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="21" outlineLevel="1">
+    <row r="416" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A416" s="5" t="s">
         <v>392</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="21" outlineLevel="1">
+    <row r="417" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A417" s="5" t="s">
         <v>392</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="21" outlineLevel="1">
+    <row r="418" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A418" s="5" t="s">
         <v>392</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="21" outlineLevel="1">
+    <row r="419" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A419" s="5" t="s">
         <v>392</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="21" outlineLevel="1">
+    <row r="420" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A420" s="5" t="s">
         <v>392</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="21" outlineLevel="1">
+    <row r="421" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A421" s="5" t="s">
         <v>392</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="21" outlineLevel="1">
+    <row r="422" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A422" s="5" t="s">
         <v>392</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="21" outlineLevel="1">
+    <row r="423" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A423" s="5" t="s">
         <v>392</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="21" outlineLevel="1">
+    <row r="424" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A424" s="5" t="s">
         <v>392</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:3" ht="21" outlineLevel="1">
+    <row r="425" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A425" s="5" t="s">
         <v>392</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="21" outlineLevel="1">
+    <row r="426" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A426" s="5" t="s">
         <v>392</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="21" outlineLevel="1">
+    <row r="427" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A427" s="5" t="s">
         <v>392</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="21" outlineLevel="1">
+    <row r="428" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A428" s="5" t="s">
         <v>392</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="21" outlineLevel="1">
+    <row r="429" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A429" s="5" t="s">
         <v>392</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="21" outlineLevel="1">
+    <row r="430" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A430" s="5" t="s">
         <v>392</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="21" outlineLevel="1">
+    <row r="431" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A431" s="5" t="s">
         <v>392</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="21" outlineLevel="1">
+    <row r="432" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A432" s="5" t="s">
         <v>392</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:3" ht="21" outlineLevel="1">
+    <row r="433" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A433" s="5" t="s">
         <v>392</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:3" ht="21" outlineLevel="1">
+    <row r="434" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A434" s="5" t="s">
         <v>392</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:3" ht="21" outlineLevel="1">
+    <row r="435" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A435" s="5" t="s">
         <v>392</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:3" ht="21" outlineLevel="1">
+    <row r="436" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A436" s="5" t="s">
         <v>392</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:3" ht="21" outlineLevel="1">
+    <row r="437" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A437" s="5" t="s">
         <v>392</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:3" ht="21" outlineLevel="1">
+    <row r="438" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A438" s="5" t="s">
         <v>392</v>
       </c>
@@ -6975,7 +6975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:3" ht="21" outlineLevel="1">
+    <row r="439" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A439" s="5" t="s">
         <v>392</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:3" ht="21" outlineLevel="1">
+    <row r="440" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A440" s="5" t="s">
         <v>392</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:3" ht="21" outlineLevel="1">
+    <row r="441" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A441" s="5" t="s">
         <v>392</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:3" ht="21" outlineLevel="1">
+    <row r="442" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A442" s="5" t="s">
         <v>392</v>
       </c>
@@ -7019,7 +7019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:3" ht="21" outlineLevel="1">
+    <row r="443" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A443" s="5" t="s">
         <v>392</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="1:3" ht="21" outlineLevel="1">
+    <row r="444" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A444" s="5" t="s">
         <v>392</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:3" ht="21" outlineLevel="1">
+    <row r="445" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A445" s="5" t="s">
         <v>392</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="1:3" ht="21" outlineLevel="1">
+    <row r="446" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A446" s="5" t="s">
         <v>392</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:3" ht="21" outlineLevel="1">
+    <row r="447" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A447" s="5" t="s">
         <v>392</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:3" ht="21" outlineLevel="1">
+    <row r="448" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A448" s="5" t="s">
         <v>392</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="1:3" ht="21" outlineLevel="1">
+    <row r="449" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A449" s="5" t="s">
         <v>392</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:3" ht="21" outlineLevel="1">
+    <row r="450" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A450" s="5" t="s">
         <v>392</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:3" ht="21" outlineLevel="1">
+    <row r="451" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A451" s="5" t="s">
         <v>392</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="1:3" ht="21" outlineLevel="1">
+    <row r="452" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A452" s="5" t="s">
         <v>392</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="1:3" ht="21" outlineLevel="1">
+    <row r="453" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A453" s="5" t="s">
         <v>392</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="1:3" ht="21" outlineLevel="1">
+    <row r="454" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A454" s="5" t="s">
         <v>392</v>
       </c>
@@ -7151,7 +7151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="455" spans="1:3" ht="21" outlineLevel="1">
+    <row r="455" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A455" s="5" t="s">
         <v>392</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="1:3" ht="21" outlineLevel="1">
+    <row r="456" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A456" s="5" t="s">
         <v>392</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="457" spans="1:3" ht="21" outlineLevel="1">
+    <row r="457" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A457" s="5" t="s">
         <v>392</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="458" spans="1:3" ht="21" outlineLevel="1">
+    <row r="458" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A458" s="5" t="s">
         <v>392</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="459" spans="1:3" ht="21" outlineLevel="1">
+    <row r="459" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A459" s="5" t="s">
         <v>392</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="460" spans="1:3" ht="21" outlineLevel="1">
+    <row r="460" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A460" s="5" t="s">
         <v>392</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="461" spans="1:3" ht="21" outlineLevel="1">
+    <row r="461" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A461" s="5" t="s">
         <v>392</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="462" spans="1:3" ht="21" outlineLevel="1">
+    <row r="462" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A462" s="5" t="s">
         <v>392</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="463" spans="1:3" ht="21" outlineLevel="1">
+    <row r="463" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A463" s="5" t="s">
         <v>392</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="464" spans="1:3" ht="21" outlineLevel="1">
+    <row r="464" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A464" s="5" t="s">
         <v>392</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="21" outlineLevel="1">
+    <row r="465" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A465" s="5" t="s">
         <v>392</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="21" outlineLevel="1">
+    <row r="466" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A466" s="5" t="s">
         <v>392</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="21" outlineLevel="1">
+    <row r="467" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A467" s="5" t="s">
         <v>392</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="468" spans="1:3" ht="21" outlineLevel="1">
+    <row r="468" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A468" s="5" t="s">
         <v>392</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="469" spans="1:3" ht="21" outlineLevel="1">
+    <row r="469" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A469" s="5" t="s">
         <v>392</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="21" outlineLevel="1">
+    <row r="470" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A470" s="5" t="s">
         <v>392</v>
       </c>
@@ -7327,16 +7327,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="471" spans="1:3" ht="21">
+    <row r="471" spans="1:3" ht="21" collapsed="1">
       <c r="B471" s="7"/>
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7451,21 +7451,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Bridges in a Graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC05A38-1EA9-4A86-BCDE-325A5F046CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065604E5-45F3-4418-8624-173CCDC624EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="C382" sqref="C382"/>
+    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
+      <selection activeCell="C383" sqref="C383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3891,11 +3891,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4393,11 +4393,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4712,11 +4712,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5108,11 +5108,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5328,11 +5328,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5757,11 +5757,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5966,11 +5966,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6321,7 +6321,7 @@
         <v>368</v>
       </c>
       <c r="C382" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D382" s="4" t="b">
         <v>0</v>
@@ -6584,11 +6584,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6661,11 +6661,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7332,11 +7332,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7451,21 +7451,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Detect Negative Cycle in a Graph
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F345F508-107D-4AA7-9014-05448242F48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F41FFFF-3D32-4B8F-834D-4FC947190E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B374" workbookViewId="0">
-      <selection activeCell="C382" sqref="C382"/>
+      <selection activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -6363,7 +6363,7 @@
         <v>371</v>
       </c>
       <c r="C385" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D385" s="4" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Detect Loop in a Single Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C79A6D-10B5-41FC-ABBF-0F2DA725C095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C29420-2D53-43FD-BA75-7958D4686A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3525,7 +3525,7 @@
         <v>137</v>
       </c>
       <c r="C142" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Detect and Delete Loop in a Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C29420-2D53-43FD-BA75-7958D4686A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9AE2B-54A3-4069-8914-4AA4A5A545E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3536,7 +3536,7 @@
         <v>138</v>
       </c>
       <c r="C143" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Remove Duplicates from a Sorted Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9AE2B-54A3-4069-8914-4AA4A5A545E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D100D180-2DDF-4B11-A3A3-B0E00CFE37EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3558,7 +3558,7 @@
         <v>140</v>
       </c>
       <c r="C145" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Remove Duplicates from an unsorted Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D100D180-2DDF-4B11-A3A3-B0E00CFE37EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F026D9FC-F465-4E68-A6A3-1FAEB06E5677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3569,7 +3569,7 @@
         <v>141</v>
       </c>
       <c r="C146" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Add “1” to a number represented as a Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F026D9FC-F465-4E68-A6A3-1FAEB06E5677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D67A18F-727A-4F91-9C76-A09BDD96B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3591,7 +3591,7 @@
         <v>143</v>
       </c>
       <c r="C148" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Add 2 numbers using Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D67A18F-727A-4F91-9C76-A09BDD96B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5278D7F0-0400-4FDD-A159-9733DFCD7183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3602,7 +3602,7 @@
         <v>144</v>
       </c>
       <c r="C149" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Intersection Of Two Sorted Linked Lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5278D7F0-0400-4FDD-A159-9733DFCD7183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3B2468-C64C-425B-853B-2C3C6E35F26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3613,7 +3613,7 @@
         <v>145</v>
       </c>
       <c r="C150" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Intersection Point in Y Shaped Linked Lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3B2468-C64C-425B-853B-2C3C6E35F26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB4257-F582-47F0-A90D-24336037D8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3624,7 +3624,7 @@
         <v>146</v>
       </c>
       <c r="C151" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Linked List is a Palindrome or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB4257-F582-47F0-A90D-24336037D8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7AC450-D059-42FD-B970-47C9D60572D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView tabSelected="1" topLeftCell="C147" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3690,7 +3690,7 @@
         <v>152</v>
       </c>
       <c r="C157" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Deletion from a Circular Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7AC450-D059-42FD-B970-47C9D60572D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0C997E-B351-44E8-BC9A-27D1ABFF7457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="10500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C147" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3701,7 +3701,7 @@
         <v>153</v>
       </c>
       <c r="C158" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Reverse a Doubly Linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0C997E-B351-44E8-BC9A-27D1ABFF7457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6F4B47-9B5F-487D-8FBF-08704A2443A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="10500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C147" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" topLeftCell="B147" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3712,7 +3712,7 @@
         <v>154</v>
       </c>
       <c r="C159" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Rotate DoublyLinked list by N nodes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6F4B47-9B5F-487D-8FBF-08704A2443A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB4367-BFBE-4632-AA44-6693B7FB19CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="10500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B147" workbookViewId="0">
-      <selection activeCell="C160" sqref="C160"/>
+    <sheetView tabSelected="1" topLeftCell="B150" workbookViewId="0">
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3756,7 +3756,7 @@
         <v>158</v>
       </c>
       <c r="C163" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Rotate a Doubly Linked list in group of Given Size
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB4367-BFBE-4632-AA44-6693B7FB19CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6812A07F-BF0B-4029-8C2F-544E564D4F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B150" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3767,7 +3767,7 @@
         <v>159</v>
       </c>
       <c r="C164" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Merge Sort for Linked Lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6812A07F-BF0B-4029-8C2F-544E564D4F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5EC52-16F1-49B7-A988-0F511F5BD99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B150" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" topLeftCell="B147" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3635,7 +3635,7 @@
         <v>147</v>
       </c>
       <c r="C152" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Quick Sort for Linked Lists
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5EC52-16F1-49B7-A988-0F511F5BD99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B868EB4-22D2-4975-B45B-505BA0B65E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B147" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="B153" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3646,7 +3646,7 @@
         <v>148</v>
       </c>
       <c r="C153" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Sort a “k”sorted Doubly Linked list
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B868EB4-22D2-4975-B45B-505BA0B65E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85002471-1BE4-42B2-800C-601D43EBBAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B153" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3745,7 +3745,7 @@
         <v>157</v>
       </c>
       <c r="C162" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="21" outlineLevel="1">
@@ -3892,11 +3892,11 @@
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4394,11 +4394,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4713,11 +4713,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5109,11 +5109,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5329,11 +5329,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5758,11 +5758,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5967,11 +5967,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6585,11 +6585,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6662,11 +6662,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7333,11 +7333,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7452,21 +7452,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Find Kth largest element in a BST
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\DSA-with-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB1637-F58A-4B0E-9999-6F0DBF10653E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C9CBC-73FE-4F4B-B4D4-004393CC45B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1726,9 +1726,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1766,7 +1766,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1872,7 +1872,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2014,7 +2014,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2024,18 +2024,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="A211" sqref="A211"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,13 +3893,13 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
-    </row>
-    <row r="178" spans="1:4" ht="21" outlineLevel="1">
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
+    </row>
+    <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="21" outlineLevel="1">
+    <row r="179" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="21" outlineLevel="1">
+    <row r="180" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="21" outlineLevel="1">
+    <row r="181" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="21" outlineLevel="1">
+    <row r="182" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="21" outlineLevel="1">
+    <row r="183" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="21" outlineLevel="1">
+    <row r="184" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="21" outlineLevel="1">
+    <row r="185" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="21" outlineLevel="1">
+    <row r="186" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="21" outlineLevel="1">
+    <row r="187" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="21" outlineLevel="1">
+    <row r="188" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="21" outlineLevel="1">
+    <row r="189" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="21" outlineLevel="1">
+    <row r="190" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="21" outlineLevel="1">
+    <row r="191" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="21" outlineLevel="1">
+    <row r="192" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="21" outlineLevel="1">
+    <row r="193" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="21" outlineLevel="1">
+    <row r="194" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="21" outlineLevel="1">
+    <row r="195" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="21" outlineLevel="1">
+    <row r="196" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="21" outlineLevel="1">
+    <row r="197" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="21" outlineLevel="1">
+    <row r="198" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="21" outlineLevel="1">
+    <row r="199" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="21" outlineLevel="1">
+    <row r="200" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="21" outlineLevel="1">
+    <row r="201" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="21" outlineLevel="1">
+    <row r="202" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="21" outlineLevel="1">
+    <row r="203" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="21" outlineLevel="1">
+    <row r="204" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="21" outlineLevel="1">
+    <row r="205" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="21" outlineLevel="1">
+    <row r="206" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="21" outlineLevel="1">
+    <row r="207" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="21" outlineLevel="1">
+    <row r="208" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="21" outlineLevel="1">
+    <row r="209" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A209" s="5" t="s">
         <v>171</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="21" outlineLevel="1">
+    <row r="210" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A210" s="5" t="s">
         <v>171</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="21" outlineLevel="1">
+    <row r="211" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A211" s="5" t="s">
         <v>171</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="21" outlineLevel="1">
+    <row r="212" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A212" s="5" t="s">
         <v>171</v>
       </c>
@@ -4389,17 +4389,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="21">
+    <row r="213" spans="1:4" ht="21" collapsed="1">
       <c r="A213" s="8"/>
       <c r="B213" s="7"/>
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4465,7 +4465,7 @@
         <v>211</v>
       </c>
       <c r="C219" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D219" s="4" t="b">
         <v>0</v>
@@ -4521,7 +4521,7 @@
         <v>215</v>
       </c>
       <c r="C223" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D223" s="4" t="b">
         <v>0</v>
@@ -4549,7 +4549,7 @@
         <v>217</v>
       </c>
       <c r="C225" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D225" s="4" t="b">
         <v>0</v>
@@ -4563,7 +4563,7 @@
         <v>218</v>
       </c>
       <c r="C226" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D226" s="4" t="b">
         <v>0</v>
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
@@ -7929,9 +7929,9 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">

</xml_diff>

<commit_message>
Find Kth smallest element in a BST
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C9CBC-73FE-4F4B-B4D4-004393CC45B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED7AF23-1ACE-4196-A027-3F4CEF91A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C225" sqref="C225"/>
+      <selection activeCell="C226" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4577,7 +4577,7 @@
         <v>219</v>
       </c>
       <c r="C227" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D227" s="4" t="b">
         <v>0</v>
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Find all conflicting appointments
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED7AF23-1ACE-4196-A027-3F4CEF91A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA28299B-DF2A-420A-A95D-382A150E2882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4647,7 +4647,7 @@
         <v>224</v>
       </c>
       <c r="C232" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D232" s="4" t="b">
         <v>0</v>
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Check preorder is valid or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA28299B-DF2A-420A-A95D-382A150E2882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742188CD-8918-4C03-96B5-77561D6E66AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4661,7 +4661,7 @@
         <v>225</v>
       </c>
       <c r="C233" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D233" s="4" t="b">
         <v>0</v>
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Check whether BST contains Dead end
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742188CD-8918-4C03-96B5-77561D6E66AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E66673D-251D-4573-AE3C-4D8B4A40BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4675,7 +4675,7 @@
         <v>226</v>
       </c>
       <c r="C234" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D234" s="4" t="b">
         <v>0</v>
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Largest BST in a Binary Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E66673D-251D-4573-AE3C-4D8B4A40BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E17A905-AC54-4E39-81B9-7231E124341B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C235" sqref="C235"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,13 +4395,13 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
-    </row>
-    <row r="215" spans="1:4" ht="21" outlineLevel="1">
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
+    </row>
+    <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
         <v>207</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="21" outlineLevel="1">
+    <row r="216" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A216" s="5" t="s">
         <v>207</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="21" outlineLevel="1">
+    <row r="217" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A217" s="5" t="s">
         <v>207</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="21" outlineLevel="1">
+    <row r="218" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A218" s="5" t="s">
         <v>207</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="21" outlineLevel="1">
+    <row r="219" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A219" s="5" t="s">
         <v>207</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="21" outlineLevel="1">
+    <row r="220" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A220" s="5" t="s">
         <v>207</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="21" outlineLevel="1">
+    <row r="221" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A221" s="5" t="s">
         <v>207</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="21" outlineLevel="1">
+    <row r="222" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A222" s="5" t="s">
         <v>207</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="21" outlineLevel="1">
+    <row r="223" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A223" s="5" t="s">
         <v>207</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="21" outlineLevel="1">
+    <row r="224" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A224" s="5" t="s">
         <v>207</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="21" outlineLevel="1">
+    <row r="225" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A225" s="5" t="s">
         <v>207</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="21" outlineLevel="1">
+    <row r="226" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A226" s="5" t="s">
         <v>207</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="21" outlineLevel="1">
+    <row r="227" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A227" s="5" t="s">
         <v>207</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="21" outlineLevel="1">
+    <row r="228" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A228" s="5" t="s">
         <v>207</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="21" outlineLevel="1">
+    <row r="229" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A229" s="5" t="s">
         <v>207</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="21" outlineLevel="1">
+    <row r="230" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A230" s="5" t="s">
         <v>207</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="21" outlineLevel="1">
+    <row r="231" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A231" s="5" t="s">
         <v>207</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="21" outlineLevel="1">
+    <row r="232" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A232" s="5" t="s">
         <v>207</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="21" outlineLevel="1">
+    <row r="233" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A233" s="5" t="s">
         <v>207</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="21" outlineLevel="1">
+    <row r="234" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A234" s="5" t="s">
         <v>207</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="21" outlineLevel="1">
+    <row r="235" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A235" s="5" t="s">
         <v>207</v>
       </c>
@@ -4689,13 +4689,13 @@
         <v>227</v>
       </c>
       <c r="C235" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D235" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="21" outlineLevel="1">
+    <row r="236" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A236" s="5" t="s">
         <v>207</v>
       </c>
@@ -4709,16 +4709,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="21">
+    <row r="237" spans="1:4" ht="21" collapsed="1">
       <c r="B237" s="7"/>
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5110,11 +5110,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:3" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5330,11 +5330,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5759,11 +5759,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -5968,11 +5968,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6586,11 +6586,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6663,11 +6663,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7334,11 +7334,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7453,21 +7453,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximum trains for which stoppage can be provided
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E6675B-ACC8-45C2-935A-396A069288C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24695D77-3662-431E-BE2B-5031A3A326E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="C244" sqref="C244"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4812,7 +4812,7 @@
         <v>236</v>
       </c>
       <c r="C245" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D245" s="4" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Find the minimum and maximum amount to buy all N candies
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278711AE-D4CE-47EC-B0F0-561AE9F7A243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC57D2F4-9291-448A-B9F6-47D76C3CFBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,16 +1680,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1701,7 +1692,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="C247" sqref="C247"/>
+      <selection activeCell="C249" sqref="C249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="27"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="23" t="s">
+      <c r="A139" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="23"/>
-      <c r="C139" s="23"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="27"/>
-      <c r="C177" s="27"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="20"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="24"/>
-      <c r="C214" s="24"/>
+      <c r="B214" s="21"/>
+      <c r="C214" s="21"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="27" t="s">
+      <c r="A238" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="27"/>
-      <c r="C238" s="27"/>
+      <c r="B238" s="20"/>
+      <c r="C238" s="20"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4854,7 +4854,7 @@
         <v>239</v>
       </c>
       <c r="C248" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D248" s="4" t="b">
         <v>0</v>
@@ -5215,11 +5215,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:4" ht="21">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="24"/>
-      <c r="C275" s="24"/>
+      <c r="B275" s="21"/>
+      <c r="C275" s="21"/>
     </row>
     <row r="276" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5435,11 +5435,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="27"/>
-      <c r="C296" s="27"/>
+      <c r="B296" s="20"/>
+      <c r="C296" s="20"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5864,11 +5864,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="24"/>
-      <c r="C336" s="24"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -6073,11 +6073,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="20" t="s">
+      <c r="A356" s="25" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="20"/>
-      <c r="C356" s="20"/>
+      <c r="B356" s="25"/>
+      <c r="C356" s="25"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6691,11 +6691,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="21" t="s">
+      <c r="A402" s="26" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="21"/>
-      <c r="C402" s="21"/>
+      <c r="B402" s="26"/>
+      <c r="C402" s="26"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6768,11 +6768,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="22" t="s">
+      <c r="A410" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="22"/>
-      <c r="C410" s="22"/>
+      <c r="B410" s="27"/>
+      <c r="C410" s="27"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7439,11 +7439,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="23" t="s">
+      <c r="A472" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="23"/>
-      <c r="C472" s="23"/>
+      <c r="B472" s="24"/>
+      <c r="C472" s="24"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7558,21 +7558,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A356:C356"/>
+    <mergeCell ref="A402:C402"/>
+    <mergeCell ref="A410:C410"/>
+    <mergeCell ref="A472:C472"/>
+    <mergeCell ref="A336:C336"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A177:C177"/>
     <mergeCell ref="A214:C214"/>
     <mergeCell ref="A238:C238"/>
     <mergeCell ref="A275:C275"/>
     <mergeCell ref="A296:C296"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A356:C356"/>
-    <mergeCell ref="A402:C402"/>
-    <mergeCell ref="A410:C410"/>
-    <mergeCell ref="A472:C472"/>
-    <mergeCell ref="A336:C336"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Find maximum meetings in one room
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE398A6B-05A0-4D1E-958D-F889B8B635F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E2A743-AF23-4F9A-B20E-57E2F26869A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B246" workbookViewId="0">
-      <selection activeCell="C252" sqref="C252"/>
+      <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4910,7 +4910,7 @@
         <v>243</v>
       </c>
       <c r="C252" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D252" s="4" t="b">
         <v>0</v>
@@ -5215,11 +5215,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:4" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5435,11 +5435,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5864,11 +5864,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -6073,11 +6073,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6691,11 +6691,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6768,11 +6768,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7439,11 +7439,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7558,21 +7558,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximize array sum after K negations
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB763514-669D-4E65-95D6-D50248127330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F043C9-515A-4526-B6E1-BD8DECBB1966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B246" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+      <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4938,7 +4938,7 @@
         <v>245</v>
       </c>
       <c r="C254" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D254" s="4" t="b">
         <v>0</v>
@@ -5215,11 +5215,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:4" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5435,11 +5435,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5864,11 +5864,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -6073,11 +6073,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6691,11 +6691,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6768,11 +6768,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7439,11 +7439,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7558,21 +7558,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
Maximize the sum of arr[i]*i
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F043C9-515A-4526-B6E1-BD8DECBB1966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44C7841-EB43-421F-9635-FD1C1C93D649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2024,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B246" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B240" workbookViewId="0">
       <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4952,7 +4952,7 @@
         <v>246</v>
       </c>
       <c r="C255" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D255" s="4" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Maximize sum of consecutive differences in a circular array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64585C7-2AFC-4352-8605-450B552A1AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9372A42-B80C-4E3A-A574-6B60863FB3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B249" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+      <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -4980,7 +4980,7 @@
         <v>248</v>
       </c>
       <c r="C257" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D257" s="4" t="b">
         <v>0</v>
@@ -5215,11 +5215,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:4" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5435,11 +5435,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5864,11 +5864,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -6073,11 +6073,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6691,11 +6691,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6768,11 +6768,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7439,11 +7439,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7558,21 +7558,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>

<commit_message>
DEFKIN -Defense of a Kingdom
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\DSA with Python\DSA-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDCA1B0-DE51-4649-AA51-D5266FEBFFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772A79D3-3E2B-4A98-8C6B-30D253434164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1680,7 +1680,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1692,16 +1701,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2025,7 +2025,7 @@
   <dimension ref="A1:F483"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="C263" sqref="C263"/>
+      <selection activeCell="C264" sqref="C264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelRow="1"/>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="F4" s="16" cm="1">
         <f t="array" ref="F4">SUM(IF(C7:C42=FALSE,1,0))+SUM(IF(C57:C99=FALSE,1,0))+SUM(IF(C45:C54=FALSE,1,0))+SUM(IF(C102:C137=FALSE,1,0))+SUM(IF(C140:C175=FALSE,1,0))+SUM(IF(C178:C212=FALSE,1,0))+SUM(IF(C215:C236=FALSE,1,0))+SUM(IF(C239:C273=FALSE,1,0))+SUM(IF(C276:C294=FALSE,1,0))+SUM(IF(C297:C334=FALSE,1,0))+SUM(IF(C337:C354=FALSE,1,0))+SUM(IF(C357:C400=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C403:C408=FALSE,1,0))+SUM(IF(C411:C470=FALSE,1,0))+SUM(IF(C473:C482=FALSE,1,0))</f>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="21">
@@ -2072,15 +2072,15 @@
       </c>
       <c r="F5" s="15" cm="1">
         <f t="array" ref="F5">SUM(IF(C7:C42=TRUE,1,0))+SUM(IF(C57:C99=TRUE,1,0))+SUM(IF(C45:C54=TRUE,1,0))+SUM(IF(C102:C137=TRUE,1,0))+SUM(IF(C140:C175=TRUE,1,0))+SUM(IF(C178:C212=TRUE,1,0))+SUM(IF(C215:C236=TRUE,1,0))+SUM(IF(C239:C273=TRUE,1,0))+SUM(IF(C276:C294=TRUE,1,0))+SUM(IF(C297:C334=TRUE,1,0))+SUM(IF(C337:C354=TRUE,1,0))+SUM(IF(C357:C400=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C403:C408=TRUE,1,0))+SUM(IF(C411:C470=TRUE,1,0))+SUM(IF(C473:C482=TRUE,1,0))</f>
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:6" ht="21" hidden="1" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="21">
-      <c r="A44" s="20" t="s">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
     </row>
     <row r="45" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A45" s="8" t="s">
@@ -2604,11 +2604,11 @@
     </row>
     <row r="55" spans="1:3" collapsed="1"/>
     <row r="56" spans="1:3" ht="21">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
     </row>
     <row r="57" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A57" s="5" t="s">
@@ -3085,11 +3085,11 @@
     </row>
     <row r="100" spans="1:3" collapsed="1"/>
     <row r="101" spans="1:3" ht="21">
-      <c r="A101" s="20" t="s">
+      <c r="A101" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="20"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
     </row>
     <row r="102" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A102" s="5" t="s">
@@ -3489,11 +3489,11 @@
     </row>
     <row r="138" spans="1:3" collapsed="1"/>
     <row r="139" spans="1:3" ht="21" customHeight="1">
-      <c r="A139" s="24" t="s">
+      <c r="A139" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
     </row>
     <row r="140" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A140" s="8" t="s">
@@ -3893,11 +3893,11 @@
     </row>
     <row r="176" spans="1:3" collapsed="1"/>
     <row r="177" spans="1:4" ht="21">
-      <c r="A177" s="20" t="s">
+      <c r="A177" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B177" s="20"/>
-      <c r="C177" s="20"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A178" s="5" t="s">
@@ -4395,11 +4395,11 @@
       <c r="C213" s="4"/>
     </row>
     <row r="214" spans="1:4" ht="21">
-      <c r="A214" s="21" t="s">
+      <c r="A214" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B214" s="21"/>
-      <c r="C214" s="21"/>
+      <c r="B214" s="24"/>
+      <c r="C214" s="24"/>
     </row>
     <row r="215" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A215" s="5" t="s">
@@ -4714,11 +4714,11 @@
       <c r="C237" s="4"/>
     </row>
     <row r="238" spans="1:4" ht="21">
-      <c r="A238" s="20" t="s">
+      <c r="A238" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B238" s="20"/>
-      <c r="C238" s="20"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:4" ht="21" outlineLevel="1">
       <c r="A239" s="5" t="s">
@@ -5064,7 +5064,7 @@
         <v>254</v>
       </c>
       <c r="C263" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D263" s="4" t="b">
         <v>0</v>
@@ -5215,11 +5215,11 @@
       <c r="C274" s="4"/>
     </row>
     <row r="275" spans="1:4" ht="21">
-      <c r="A275" s="21" t="s">
+      <c r="A275" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="B275" s="21"/>
-      <c r="C275" s="21"/>
+      <c r="B275" s="24"/>
+      <c r="C275" s="24"/>
     </row>
     <row r="276" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A276" s="5" t="s">
@@ -5435,11 +5435,11 @@
       <c r="C295" s="4"/>
     </row>
     <row r="296" spans="1:3" ht="21">
-      <c r="A296" s="20" t="s">
+      <c r="A296" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B296" s="20"/>
-      <c r="C296" s="20"/>
+      <c r="B296" s="27"/>
+      <c r="C296" s="27"/>
     </row>
     <row r="297" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A297" s="5" t="s">
@@ -5864,11 +5864,11 @@
       <c r="C335" s="4"/>
     </row>
     <row r="336" spans="1:3" ht="21">
-      <c r="A336" s="21" t="s">
+      <c r="A336" s="24" t="s">
         <v>323</v>
       </c>
-      <c r="B336" s="21"/>
-      <c r="C336" s="21"/>
+      <c r="B336" s="24"/>
+      <c r="C336" s="24"/>
     </row>
     <row r="337" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A337" s="8" t="s">
@@ -6073,11 +6073,11 @@
       <c r="C355" s="4"/>
     </row>
     <row r="356" spans="1:4" ht="21" customHeight="1">
-      <c r="A356" s="25" t="s">
+      <c r="A356" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="B356" s="25"/>
-      <c r="C356" s="25"/>
+      <c r="B356" s="20"/>
+      <c r="C356" s="20"/>
     </row>
     <row r="357" spans="1:4" ht="21" hidden="1" outlineLevel="1">
       <c r="A357" s="8" t="s">
@@ -6691,11 +6691,11 @@
       <c r="C401" s="4"/>
     </row>
     <row r="402" spans="1:3" ht="21" customHeight="1">
-      <c r="A402" s="26" t="s">
+      <c r="A402" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="B402" s="26"/>
-      <c r="C402" s="26"/>
+      <c r="B402" s="21"/>
+      <c r="C402" s="21"/>
     </row>
     <row r="403" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A403" s="8" t="s">
@@ -6768,11 +6768,11 @@
       <c r="C409" s="4"/>
     </row>
     <row r="410" spans="1:3" ht="21" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B410" s="27"/>
-      <c r="C410" s="27"/>
+      <c r="B410" s="22"/>
+      <c r="C410" s="22"/>
     </row>
     <row r="411" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A411" s="5" t="s">
@@ -7439,11 +7439,11 @@
       <c r="C471" s="4"/>
     </row>
     <row r="472" spans="1:3" ht="21" customHeight="1">
-      <c r="A472" s="24" t="s">
+      <c r="A472" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="B472" s="24"/>
-      <c r="C472" s="24"/>
+      <c r="B472" s="23"/>
+      <c r="C472" s="23"/>
     </row>
     <row r="473" spans="1:3" ht="21" hidden="1" outlineLevel="1">
       <c r="A473" s="5" t="s">
@@ -7558,21 +7558,21 @@
     <row r="483" spans="1:3" collapsed="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A177:C177"/>
+    <mergeCell ref="A214:C214"/>
+    <mergeCell ref="A238:C238"/>
+    <mergeCell ref="A275:C275"/>
+    <mergeCell ref="A296:C296"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A139:C139"/>
     <mergeCell ref="A356:C356"/>
     <mergeCell ref="A402:C402"/>
     <mergeCell ref="A410:C410"/>
     <mergeCell ref="A472:C472"/>
     <mergeCell ref="A336:C336"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="A139:C139"/>
-    <mergeCell ref="A177:C177"/>
-    <mergeCell ref="A214:C214"/>
-    <mergeCell ref="A238:C238"/>
-    <mergeCell ref="A275:C275"/>
-    <mergeCell ref="A296:C296"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>

</xml_diff>